<commit_message>
Stage 2 A7-A20 Stage 3 B1-B2
</commit_message>
<xml_diff>
--- a/N1ghtSe7en/evidence.xlsx
+++ b/N1ghtSe7en/evidence.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Валерчик\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Валерчик\Desktop\крипта\Cosmos\GoN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B82CA4C1-81C7-4EF1-AC88-E7CCA6C39A67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1935FF22-F32A-4794-AF1D-BE38098E3EF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="90">
   <si>
     <t>TxHash</t>
   </si>
@@ -58,27 +58,12 @@
     <t>ChainID</t>
   </si>
   <si>
-    <t>tx hash on that chain</t>
-  </si>
-  <si>
-    <t>chain id</t>
-  </si>
-  <si>
-    <t>tx hash on that chain	chain id</t>
-  </si>
-  <si>
     <t>ClassID</t>
   </si>
   <si>
     <t>NFTID</t>
   </si>
   <si>
-    <t>ibc class on chain</t>
-  </si>
-  <si>
-    <t>nft id</t>
-  </si>
-  <si>
     <t>TeamName</t>
   </si>
   <si>
@@ -167,13 +152,175 @@
   </si>
   <si>
     <t>DB7C82016AC1620078ED859B09F4E1A9DAEDA79718A775A1C9B99E05038768CE</t>
+  </si>
+  <si>
+    <t>ibc/17627F3D72A7A91C1F1F4FEFE8175078C780318CED8BDE638DF82AD8A35D5457</t>
+  </si>
+  <si>
+    <t>n7a7</t>
+  </si>
+  <si>
+    <t>n7a8</t>
+  </si>
+  <si>
+    <t>ibc/F8010DECCE4E20E01EB22CFB39C7B0C96F9BA77D25CEC4E96DFC8436D699B2DF</t>
+  </si>
+  <si>
+    <t>ibc/17695DC202304B1B1099965B9E522E389A160D7065C2EFA719BF16C4CE6F25C3</t>
+  </si>
+  <si>
+    <t>n7a91</t>
+  </si>
+  <si>
+    <t>ibc/760F0825E0F9414AFE55B49C678B6A4941F3B80D1607F7179D3EA98A548FF640</t>
+  </si>
+  <si>
+    <t>n7a11</t>
+  </si>
+  <si>
+    <t>83A937F905652AA5FA4C7F90CCFEA2E167E4C20E6E255A43E28FE7B79EAA871D</t>
+  </si>
+  <si>
+    <t>gon-irishub-1</t>
+  </si>
+  <si>
+    <t>FE130FD240C07C8DF735C4F7AA89B9D7B22BFB74827663C686663D8DDBE1FFF5</t>
+  </si>
+  <si>
+    <t>uptick_7000-2</t>
+  </si>
+  <si>
+    <t>88D5B8F6DB61C35301803B70646B0621DECC50683600F94A6D8D2B76DCACA1F6</t>
+  </si>
+  <si>
+    <t>3D19703B26C93AE7E1FBD21EEB10AEBC4603E6F4F187AA619E92182937AA62C3</t>
+  </si>
+  <si>
+    <t>ibc/E6A322492E44B1DF0C799B603BFC24481D2F46BE5EABB281FAB5F7BCEC26B57F</t>
+  </si>
+  <si>
+    <t>n7a102</t>
+  </si>
+  <si>
+    <t>ibc/4D56EC620612074E5A698F59575DB97F5BA1BEB017ED27D376EA593BA1E72B00</t>
+  </si>
+  <si>
+    <t>n7a121</t>
+  </si>
+  <si>
+    <t>B225C235EE430D511E07EE060D6062C6360C336501658F20439734D00D49C3D3</t>
+  </si>
+  <si>
+    <t>2FA31383B20891DC8050DE56AD05BFE878FA2B35A39767C1817E8441038AC4CD</t>
+  </si>
+  <si>
+    <t>elgafar-1</t>
+  </si>
+  <si>
+    <t>AA2E3221B8C0CE92ACC7D07AB96591F4C016BDBD15E0642E9CD1276C06B60133</t>
+  </si>
+  <si>
+    <t>C919AB92FA8260DCF554E72FB7F3CB40A43BC57968637CF7EE363CB5EC02408F</t>
+  </si>
+  <si>
+    <t>60D8CA8AF170F4F57AAC59A2026C7E06EB164E0A6EF32CFC4D1F03734F9EADA3</t>
+  </si>
+  <si>
+    <t>0027C72096AC8E87063005FECEB31743650B908E3D67C80D629F09A639BF2E93</t>
+  </si>
+  <si>
+    <t>D64DA58CE92631CDA7217A81C1177C85F6253CF2189D79AC15893B9CF556966B</t>
+  </si>
+  <si>
+    <t>95D6342E02A64E1C19496719CEBB13F955CD63F7F56866F95D69DA74E4244D97</t>
+  </si>
+  <si>
+    <t>4DCD4BE3831C7873A4B472ED3360C2B7D46F064E96140D9DF9FDE4EBAB5ED2BC</t>
+  </si>
+  <si>
+    <t>1B821A4E82E559870FD63906F807EF1EB9F2C5C15809124011449703FAF8A124</t>
+  </si>
+  <si>
+    <t>F5B301E7B3C8CC26C80043ECA47C7160A1929EAAC75B0537B46023AB82DAC427</t>
+  </si>
+  <si>
+    <t>712FCD0C016C4FCCC23746A1634E8E4CFCCE19ADEC6B4E71F93FD0E1D0BB8F3C</t>
+  </si>
+  <si>
+    <t>9A6AF12E9F4D7C6563F40A77E65DD0046BA78CF36C8B10C05D72ACDDE6FBDB8E</t>
+  </si>
+  <si>
+    <t>BACA6A33F897C5782BD9D2810AE08FC8FEE64D4BF693421553AEEE69C55130DB</t>
+  </si>
+  <si>
+    <t>C05AE104E5C4542C59A6AC08AE7F0F0A5894FF485E7773F6E32B2A834505E7F1</t>
+  </si>
+  <si>
+    <t>2415C80CCC7C804FEF60DD3BD33C2BC54852A48E8147321668BEB6207C979DF9</t>
+  </si>
+  <si>
+    <t>A60C4CA9836A3E3B6EB5C3C6808F8E906D46D1C6F82C0A0C64B0C12EB5C3822F</t>
+  </si>
+  <si>
+    <t>911AE86EFEFBD23E148594B87EF14B6B441397F778E0961E36ED48BC7C9E8151</t>
+  </si>
+  <si>
+    <t>D9206AD13C79E8F6024BBBC7A38A2D677CCDAC6DC0351BEB14A09EB6304D15C9</t>
+  </si>
+  <si>
+    <t>A5D2F0384CF2B10BEF74E40C0A2117E7DE116AF7E606DB5A0464FBF0ABE76283</t>
+  </si>
+  <si>
+    <t>DEA4BCE5001ED2783878ED6EF723F4832B713ABEB5A714C6704003ABFF072187</t>
+  </si>
+  <si>
+    <t>5CE9329BEBB784915B7AA70E5F6668D0D9ACCB9465749DF5C798AEFB7E5D3C8B</t>
+  </si>
+  <si>
+    <t>F22736A14170D33DDC4C4EF3389D165391AE2824CA76482BD7C5DD4749797DAA</t>
+  </si>
+  <si>
+    <t>77890909316268A2457466BAA0B169D6142ADBB4FC240C5C82E85B627C2D0C20</t>
+  </si>
+  <si>
+    <t>DF64C8C63B4E2D4CEFBE82FA5EE21FC42FC66F5589C2B30BBB56F66353DEBC36</t>
+  </si>
+  <si>
+    <t>DB7F90B849A3A7C4EE7DAC7AC01C9D93DF9018E7D54618012FCC961848BD4AFC</t>
+  </si>
+  <si>
+    <t>676D00335AC3B3E32A2AC0676F31D07FD832A74284BF07EB0B079F05989891DB</t>
+  </si>
+  <si>
+    <t>B72BEDE54A8D0F8A98C2503808962EE5A12134196419AD7D30679176EC42F395</t>
+  </si>
+  <si>
+    <t>60A12AB360BB17D3A240FF1823F8C68789A936A89BC61014D1D26AE1D03CB1E4</t>
+  </si>
+  <si>
+    <t>171A4B74F34BB2CD144595A72CFA66BD634FF8C3AE2E40DE57C726F473BE8FED</t>
+  </si>
+  <si>
+    <t>521122A917440AE333C4B1D51AB574CA912A60979E2D79D90EED12E749A18BD3</t>
+  </si>
+  <si>
+    <t>26B6779F04CCDEB7380D253BA2B081B995FE4679F86C342B5108AC347D5F99AC</t>
+  </si>
+  <si>
+    <t>35E8D3B7793830A05499E2CC9503ECD4531390E35858E340A2B8D43F683CF6CF</t>
+  </si>
+  <si>
+    <t>C4B7343D32CB332B9B05D51BBE79EBA20EADE0BCF6988CB7B5371B32114221D0</t>
+  </si>
+  <si>
+    <t>40732B9482029A142A654B075C04A576F426B72B1FBDCC3DDF51BF0366A8057E</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -187,8 +334,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF24292F"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+      <charset val="204"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -203,6 +357,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -240,7 +400,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -255,6 +415,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -581,54 +748,54 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="F2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -643,7 +810,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -653,18 +822,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -679,7 +848,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -689,18 +860,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -715,7 +886,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -725,18 +898,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -751,7 +924,9 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -761,18 +936,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>52</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -785,9 +960,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -805,26 +982,39 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>54</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>55</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+        <v>57</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -833,9 +1023,74 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9" style="3" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" copies="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -853,37 +1108,51 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>59</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>60</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+        <v>61</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -901,42 +1170,56 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>63</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>64</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+        <v>65</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -949,42 +1232,56 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>67</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>68</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+        <v>69</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -997,42 +1294,94 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>71</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>72</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+        <v>73</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="82.28515625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1045,80 +1394,72 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>75</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>76</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
+        <v>77</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="82.28515625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1131,71 +1472,51 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>81</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>82</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4"/>
-    </row>
-    <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4"/>
+        <v>83</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>47</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1209,6 +1530,78 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1221,7 +1614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1236,8 +1629,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1270,74 +1663,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:A3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
@@ -1360,32 +1685,32 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1400,7 +1725,7 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1416,10 +1741,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1427,16 +1752,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1467,10 +1792,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1478,16 +1803,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1518,10 +1843,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1529,16 +1854,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1553,7 +1878,7 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -1570,10 +1895,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -1581,31 +1906,71 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1615,54 +1980,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>